<commit_message>
updated metadata and notes
</commit_message>
<xml_diff>
--- a/metadata/metadata_ALCL_Thymus_RLN.xlsx
+++ b/metadata/metadata_ALCL_Thymus_RLN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/putriramadani/Documents/GitHub/scRNAseq_ALCL_Thymus_RLN/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03256797-09DE-9042-9C05-F8B0E35725FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F87585-8325-B747-BE81-50B5A151FDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22700" windowHeight="17680" xr2:uid="{5D30E324-5690-4D49-86CB-3AC4238AD353}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="181">
   <si>
     <t>Sample</t>
   </si>
@@ -576,6 +576,9 @@
   </si>
   <si>
     <t>Thymus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -980,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B13C7E-0E5C-AA46-9AFB-DB0824ACFBC2}">
-  <dimension ref="A1:AT20"/>
+  <dimension ref="A1:AT30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="AF24" sqref="AF24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2130,7 +2133,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>170</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>171</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>172</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>173</v>
       </c>
@@ -2184,6 +2187,11 @@
       </c>
       <c r="K20" s="5" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AR30" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>